<commit_message>
Added method for insert data to namedRange
</commit_message>
<xml_diff>
--- a/NamedRangeTestApp/Data/testExcel.xlsx
+++ b/NamedRangeTestApp/Data/testExcel.xlsx
@@ -1,74 +1,97 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\NamedRangeTestApp\NamedRangeTestApp\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\NamedRangeTestApp\NamedRangeTestApp\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66057BC5-FBB4-453C-A88C-CF1AD3B3A35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="test">Лист1!$G$10:$I$12</definedName>
-    <definedName name="TestRange">Лист1!$C$11:$E$13</definedName>
-    <definedName name="TestRange1">Лист1!$B$2:$F$7</definedName>
+    <definedName name="test">'Лист1'!$G$10:$I$12</definedName>
+    <definedName name="TestRange">'Лист1'!$C$11:$E$13</definedName>
+    <definedName name="TestRange1">'Лист1'!$B$2:$F$7</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>d</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>QWE</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>ASD</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -92,11 +115,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -373,151 +397,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2">
+    <row r="2">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2">
+    </row>
+    <row r="3">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3">
+    <row r="11">
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+    </row>
+    <row r="12">
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
+      <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
+      <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3">
+    </row>
+    <row r="13">
+      <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
+      <c r="E13" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D4">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>14</v>
-      </c>
-      <c r="F4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>17</v>
-      </c>
-      <c r="D5">
-        <v>18</v>
-      </c>
-      <c r="E5">
-        <v>19</v>
-      </c>
-      <c r="F5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>21</v>
-      </c>
-      <c r="C6">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>23</v>
-      </c>
-      <c r="E6">
-        <v>24</v>
-      </c>
-      <c r="F6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>26</v>
-      </c>
-      <c r="C7">
-        <v>27</v>
-      </c>
-      <c r="D7">
-        <v>28</v>
-      </c>
-      <c r="E7">
-        <v>29</v>
-      </c>
-      <c r="F7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>